<commit_message>
add faiss speed and reranker
</commit_message>
<xml_diff>
--- a/output_result/news_data_with_topics.xlsx
+++ b/output_result/news_data_with_topics.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>{"A股首例市值退市股即将摘牌": {"topic": "金融", "similarity": 0.38118407130241394}, "9月1日晚间，*ST深天（000023，股价：1.72元": {"topic": "金融", "similarity": 0.3756154179573059}, "总市值2.387亿元）公告称，公司股票已被深圳证券交易所决定终止上市，并将于2024年9月2日摘牌": {"topic": "金融", "similarity": 0.3806456923484802}, "公告显示，6月27日至7月24日，*ST深天通过深交所交易系统连续二十个交易日的股票收盘市值均低于3亿元，触及深交所《股票上市规则(2023年8月修订)》第9.2.1条第一款第六项规定的股票终止上市情形": {"topic": "金融", "similarity": 0.38248902559280396}, "值得注意的是，*ST深天此番退市，为A股公司市值退市首例，创造A股市场新的历史": {"topic": "金融", "similarity": 0.43219250440597534}, "根据目前仍在执行的规定，公司连续二十个交易日在深交所的股票收盘市值均低于3亿元，深交所终止其股票上市交易": {"topic": "金融", "similarity": 0.4240325391292572}, "而根据深交所此前发布的《深圳证券交易所股票上市规则（2024年修订）》，如果A股公司“连续二十个交易日在本所的股票收盘总市值均低于5亿元”，就会被终止上市，关于市值退市情形的修订将自2024年10月30日起计算相关期限，意味着未来上市公司触及市值退市的概率会更高": {"topic": "金融", "similarity": 0.4884668290615082}, "*ST深天是一家以商品混凝土为主业、房地产为支柱产业的上市公司，主要产业包括商品混凝土的生产和销售、房地产的开发及物业管理等": {"topic": "金融", "similarity": 0.4347127676010132}, "据*ST深天披露，2024年上半年，受地产行业需求下滑影响，深圳市和株洲市混凝土行业内生产能力的过剩更加严重，导致市场竞争更加激烈": {"topic": "生产投资", "similarity": 0.38215765357017517}, "公司混凝土业务受市场需求不足、公司资金压力加大等不利因素的影响，企业运行艰难程度不断增加": {"topic": "房地产", "similarity": 0.3702734410762787}, "在房地产板块，*ST深天1984年起涉足房地产业，与其他公司合作开发了一批商住楼宇": {"topic": "房地产", "similarity": 0.4215206801891327}, "而后公司设立专门从事房地产开发与经营的工程开发公司，自成立以来，先后开发了数个住宅、工业、商业物业": {"topic": "房地产", "similarity": 0.4694921374320984}, "公司现有房地产业务主要以商用物业及普通住宅为主，业务区域主要集中在深圳、西安和连云港": {"topic": "房地产", "similarity": 0.5097490549087524}, "值得注意的是，8月30日，*ST深天还公告表示，公司决定起诉公司控股股东广东君浩股权投资控股有限公司和实际控制人林宏润": {"topic": "金融", "similarity": 0.4017888307571411}, "2023年4月30日，*ST深天全资子公司深圳市天地顺铭企业管理有限公司（下称“天地顺铭”）与深圳市乾闳贸易有限公司签订了水泥矿粉砂石《购销合同》，2023年5月4日，天地顺铭以预付款形式将其渤海银行股份有限公司北京万寿路支行账户1.37亿元转入深圳市乾闳贸易有限公司": {"topic": "金融", "similarity": 0.37965908646583557}, "每日经济新闻综合上市公司公告（文章来源：每日经济新闻）": {"topic": "金融", "similarity": 0.3918023109436035}}</t>
+          <t>{"A股首例市值退市股即将摘牌": {"topic": "金融", "similarity": 0.3811839818954468, "prompt": "新闻文本是A股首例市值退市股即将摘牌，包含的情绪词典是stock：0.0，stockpile：0.1"}, "9月1日晚间，*ST深天（000023，股价：1.72元": {"topic": "金融", "similarity": 0.37561529874801636, "prompt": "新闻文本是9月1日晚间，*ST深天（000023，股价：1.72元，包含的情绪词典是deeper：-0.2，deepen：-0.2"}, "总市值2.387亿元）公告称，公司股票已被深圳证券交易所决定终止上市，并将于2024年9月2日摘牌": {"topic": "金融", "similarity": 0.3806457221508026, "prompt": "新闻文本是总市值2.387亿元）公告称，公司股票已被深圳证券交易所决定终止上市，并将于2024年9月2日摘牌，包含的情绪词典是terminate：-0.5，stock：0.0"}, "公告显示，6月27日至7月24日，*ST深天通过深交所交易系统连续二十个交易日的股票收盘市值均低于3亿元，触及深交所《股票上市规则(2023年8月修订)》第9.2.1条第一款第六项规定的股票终止上市情形": {"topic": "金融", "similarity": 0.38248908519744873, "prompt": "新闻文本是公告显示，6月27日至7月24日，*ST深天通过深交所交易系统连续二十个交易日的股票收盘市值均低于3亿元，触及深交所《股票上市规则(2023年8月修订)》第9.2.1条第一款第六项规定的股票终止上市情形，包含的情绪词典是stock：0.0，stop：0.0"}, "根据深交所《股票上市规则(2024年修订)》第9.2.7条的规定以及深交所上市审核委员会的审议意见，深交所决定终止公司股票上市": {"topic": null, "similarity": null, "prompt": "新闻文本是根据深交所《股票上市规则(2024年修订)》第9.2.7条的规定以及深交所上市审核委员会的审议意见，深交所决定终止公司股票上市，包含的情绪词典是stock：0.0，stop：0.0"}, "同时，根据相关规定，公司股票因触及交易类强制退市情形被作出终止上市决定，不进入退市整理期": {"topic": null, "similarity": null, "prompt": "新闻文本是同时，根据相关规定，公司股票因触及交易类强制退市情形被作出终止上市决定，不进入退市整理期，包含的情绪词典是stock：0.0，cancellation：-0.4"}, "值得注意的是，*ST深天此番退市，为A股公司市值退市首例，创造A股市场新的历史": {"topic": "金融", "similarity": 0.4321923851966858, "prompt": "新闻文本是值得注意的是，*ST深天此番退市，为A股公司市值退市首例，创造A股市场新的历史，包含的情绪词典是stock：0.0，deeper：-0.2"}, "根据目前仍在执行的规定，公司连续二十个交易日在深交所的股票收盘市值均低于3亿元，深交所终止其股票上市交易": {"topic": "金融", "similarity": 0.4240325093269348, "prompt": "新闻文本是根据目前仍在执行的规定，公司连续二十个交易日在深交所的股票收盘市值均低于3亿元，深交所终止其股票上市交易，包含的情绪词典是stock：0.0，limitation：-0.3"}, "而根据深交所此前发布的《深圳证券交易所股票上市规则（2024年修订）》，如果A股公司“连续二十个交易日在本所的股票收盘总市值均低于5亿元”，就会被终止上市，关于市值退市情形的修订将自2024年10月30日起计算相关期限，意味着未来上市公司触及市值退市的概率会更高": {"topic": "金融", "similarity": 0.48846685886383057, "prompt": "新闻文本是而根据深交所此前发布的《深圳证券交易所股票上市规则（2024年修订）》，如果A股公司“连续二十个交易日在本所的股票收盘总市值均低于5亿元”，就会被终止上市，关于市值退市情形的修订将自2024年10月30日起计算相关期限，意味着未来上市公司触及市值退市的概率会更高，包含的情绪词典是stock：0.0，limit：-0.1"}, "*ST深天是一家以商品混凝土为主业、房地产为支柱产业的上市公司，主要产业包括商品混凝土的生产和销售、房地产的开发及物业管理等": {"topic": "金融", "similarity": 0.4347127079963684, "prompt": "新闻文本是*ST深天是一家以商品混凝土为主业、房地产为支柱产业的上市公司，主要产业包括商品混凝土的生产和销售、房地产的开发及物业管理等，包含的情绪词典是deep：-0.2，enterprise：0.0"}, "2020年起，*ST深天业绩就持续呈现亏损局面": {"topic": null, "similarity": null, "prompt": "新闻文本是2020年起，*ST深天业绩就持续呈现亏损局面，包含的情绪词典是stock：0.0，deep：-0.2"}, "2024年上半年，该公司亏损额已经超越营收规模，实现营业收入4083.54万元，同比下滑54.35%": {"topic": null, "similarity": null, "prompt": "新闻文本是2024年上半年，该公司亏损额已经超越营收规模，实现营业收入4083.54万元，同比下滑54.35%，包含的情绪词典是loss：-0.7，profitability：0.6"}, "净利润亏损7032.84万元": {"topic": null, "similarity": null, "prompt": "新闻文本是净利润亏损7032.84万元，包含的情绪词典是profitability：0.6，profit：0.8"}, "据*ST深天披露，2024年上半年，受地产行业需求下滑影响，深圳市和株洲市混凝土行业内生产能力的过剩更加严重，导致市场竞争更加激烈": {"topic": "生产投资", "similarity": 0.38215774297714233, "prompt": "新闻文本是据*ST深天披露，2024年上半年，受地产行业需求下滑影响，深圳市和株洲市混凝土行业内生产能力的过剩更加严重，导致市场竞争更加激烈，包含的情绪词典是deep：-0.2，industry：0.0"}, "公司混凝土业务受市场需求不足、公司资金压力加大等不利因素的影响，企业运行艰难程度不断增加": {"topic": "房地产", "similarity": 0.37027350068092346, "prompt": "新闻文本是公司混凝土业务受市场需求不足、公司资金压力加大等不利因素的影响，企业运行艰难程度不断增加，包含的情绪词典是stress：-0.5，stressed：-0.5"}, "在房地产板块，*ST深天1984年起涉足房地产业，与其他公司合作开发了一批商住楼宇": {"topic": "房地产", "similarity": 0.4215207099914551, "prompt": "新闻文本是在房地产板块，*ST深天1984年起涉足房地产业，与其他公司合作开发了一批商住楼宇，包含的情绪词典是industry：0.0，investment：0.4"}, "而后公司设立专门从事房地产开发与经营的工程开发公司，自成立以来，先后开发了数个住宅、工业、商业物业": {"topic": "房地产", "similarity": 0.4694921672344208, "prompt": "新闻文本是而后公司设立专门从事房地产开发与经营的工程开发公司，自成立以来，先后开发了数个住宅、工业、商业物业，包含的情绪词典是development：0.4，company：0.0"}, "公司现有房地产业务主要以商用物业及普通住宅为主，业务区域主要集中在深圳、西安和连云港": {"topic": "房地产", "similarity": 0.5097491145133972, "prompt": "新闻文本是公司现有房地产业务主要以商用物业及普通住宅为主，业务区域主要集中在深圳、西安和连云港，包含的情绪词典是company：0.0，corporate：0.0"}, "值得注意的是，8月30日，*ST深天还公告表示，公司决定起诉公司控股股东广东君浩股权投资控股有限公司和实际控制人林宏润": {"topic": "金融", "similarity": 0.4017888903617859, "prompt": "新闻文本是值得注意的是，8月30日，*ST深天还公告表示，公司决定起诉公司控股股东广东君浩股权投资控股有限公司和实际控制人林宏润，包含的情绪词典是investor：0.4，deep：-0.2"}, "2023年4月30日，*ST深天全资子公司深圳市天地顺铭企业管理有限公司（下称“天地顺铭”）与深圳市乾闳贸易有限公司签订了水泥矿粉砂石《购销合同》，2023年5月4日，天地顺铭以预付款形式将其渤海银行股份有限公司北京万寿路支行账户1.37亿元转入深圳市乾闳贸易有限公司": {"topic": "金融", "similarity": 0.37965911626815796, "prompt": "新闻文本是2023年4月30日，*ST深天全资子公司深圳市天地顺铭企业管理有限公司（下称“天地顺铭”）与深圳市乾闳贸易有限公司签订了水泥矿粉砂石《购销合同》，2023年5月4日，天地顺铭以预付款形式将其渤海银行股份有限公司北京万寿路支行账户1.37亿元转入深圳市乾闳贸易有限公司，包含的情绪词典是trading：0.0，investment：0.4"}, "以预付材料款的名义形成非经营性资金占用1.37亿元": {"topic": null, "similarity": null, "prompt": "新闻文本是以预付材料款的名义形成非经营性资金占用1.37亿元，包含的情绪词典是investment：0.4，money：0.2"}, "截至2023年8月28日，累计非经营性资金占用余额1.37亿元": {"topic": null, "similarity": null, "prompt": "新闻文本是截至2023年8月28日，累计非经营性资金占用余额1.37亿元，包含的情绪词典是money：0.2，financial：0.0"}, "经公司实际控制人林宏润及控股股东确认，上述合同及资金往来没有实质性交易，控股股东广东君浩借此形成1.37亿元的往来款用于归还其债务，构成控股股东对深天地的非经营性资金占用": {"topic": null, "similarity": null, "prompt": "新闻文本是经公司实际控制人林宏润及控股股东确认，上述合同及资金往来没有实质性交易，控股股东广东君浩借此形成1.37亿元的往来款用于归还其债务，构成控股股东对深天地的非经营性资金占用，包含的情绪词典是financial：0.0，investment：0.4"}, "截至公告披露日，*ST深天暂未收到实际控制人、控股股东明确、可执行的还款措施，暂无还款保障措施和具体的还款方案，广东君浩对上市公司的非经营性资金占用余额仍为1.37亿元": {"topic": null, "similarity": null, "prompt": "新闻文本是截至公告披露日，*ST深天暂未收到实际控制人、控股股东明确、可执行的还款措施，暂无还款保障措施和具体的还款方案，广东君浩对上市公司的非经营性资金占用余额仍为1.37亿元，包含的情绪词典是financial：0.0，finance：0.0"}, "每日经济新闻综合上市公司公告（文章来源：每日经济新闻）": {"topic": "金融", "similarity": 0.39180225133895874, "prompt": "新闻文本是每日经济新闻综合上市公司公告（文章来源：每日经济新闻），包含的情绪词典是economic：0.0，stock：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -588,7 +588,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>{"值得一提的是，8月以来已有大胜达（603687.SH）、徕木股份（603633.SH）先后发布留置公告，上述消息发布后两家公司次日股价均以跌停收盘": {"topic": "金融", "similarity": 0.3826305866241455}}</t>
+          <t>{"又见A股上市公司实控人被留置，涉事公司分别是半导体设备供应商耐科装备（688419.SH）和知名中药公司*ST大药(603963.SH)": {"topic": null, "similarity": null, "prompt": "新闻文本是又见A股上市公司实控人被留置，涉事公司分别是半导体设备供应商耐科装备（688419.SH）和知名中药公司*ST大药(603963.SH)，包含的情绪词典是stock：0.0，stay：0.0"}, "8月30日盘后，耐科装备发布公告称，公司于2024年8月30日收到公司实际控制人之一、董事长、法定代表人黄明玖家属的通知，黄明玖家属于2024年8月29日收到铜陵市铜官区监察委员会签发的《留置通知书》和《立案通知书》，黄明玖被实施留置并立案调查": {"topic": null, "similarity": null, "prompt": "新闻文本是8月30日盘后，耐科装备发布公告称，公司于2024年8月30日收到公司实际控制人之一、董事长、法定代表人黄明玖家属的通知，黄明玖家属于2024年8月29日收到铜陵市铜官区监察委员会签发的《留置通知书》和《立案通知书》，黄明玖被实施留置并立案调查，包含的情绪词典是hardship：-0.5，corporate：0.0"}, "对于本次黄明玖被实施留置并立案调查事宜，耐科装备表示，将按照《公司法》、《上市公司治理准则》等法律法规和相关制度规范运作，日常经营管理由高管团队负责，高管团队已针对相关事项做了妥善安排": {"topic": null, "similarity": null, "prompt": "新闻文本是对于本次黄明玖被实施留置并立案调查事宜，耐科装备表示，将按照《公司法》、《上市公司治理准则》等法律法规和相关制度规范运作，日常经营管理由高管团队负责，高管团队已针对相关事项做了妥善安排，包含的情绪词典是corporate：0.0，hardship：-0.5"}, "“截至本公告披露日，公司控制权未发生变化，董事会运作正常，生产经营管理情况正常，本事项不会对公司正常生产经营产生重大影响": {"topic": null, "similarity": null, "prompt": "新闻文本是“截至本公告披露日，公司控制权未发生变化，董事会运作正常，生产经营管理情况正常，本事项不会对公司正常生产经营产生重大影响，包含的情绪词典是company：0.0，corporate：0.0"}, "”耐科装备表示，“公司尚未知悉立案调查的进展及结论，将持续关注上述事项的后续情况，并及时履行信息披露义务、提示相关风险": {"topic": null, "similarity": null, "prompt": "新闻文本是”耐科装备表示，“公司尚未知悉立案调查的进展及结论，将持续关注上述事项的后续情况，并及时履行信息披露义务、提示相关风险，包含的情绪词典是company：0.0，could：0.0"}, "” 　　耐科装备2023年年报显示，公司股权相对分散，目前无控股股东，实际控制人为黄明玖、郑天勤、吴成胜、徐劲风、胡火根五人组成的一致行动人，合计直接持有公司29.05%的股份": {"topic": null, "similarity": null, "prompt": "新闻文本是” 　　耐科装备2023年年报显示，公司股权相对分散，目前无控股股东，实际控制人为黄明玖、郑天勤、吴成胜、徐劲风、胡火根五人组成的一致行动人，合计直接持有公司29.05%的股份，包含的情绪词典是corporate：0.0，company：0.0"}, "年报信息还显示，黄明玖，1962年生，中国国籍，无境外永久居留权，所学专业为工模具设计与制造，后取得工商管理专业硕士学历，工程师，全面负责耐科装备研发工作，其中作为主要发明人申请并取得了多项专利": {"topic": null, "similarity": null, "prompt": "新闻文本是年报信息还显示，黄明玖，1962年生，中国国籍，无境外永久居留权，所学专业为工模具设计与制造，后取得工商管理专业硕士学历，工程师，全面负责耐科装备研发工作，其中作为主要发明人申请并取得了多项专利，包含的情绪词典是engineering：0.0，industrial：0.0"}, "图片来源：耐科装备公告截图　　*ST大药9月1日公告，公司与实际控制人、董事长兼总经理杨君祥家属于2024年8月31日收到由镇康县监察委员会签发的杨君祥被留置、立案调查的通知书": {"topic": null, "similarity": null, "prompt": "新闻文本是图片来源：耐科装备公告截图　　*ST大药9月1日公告，公司与实际控制人、董事长兼总经理杨君祥家属于2024年8月31日收到由镇康县监察委员会签发的杨君祥被留置、立案调查的通知书，包含的情绪词典是corporate：0.0，stock：0.0"}, "*ST大药表示，“所涉事项与公司无关，截至本公告披露日，公司未被相关机关要求协助调查": {"topic": null, "similarity": null, "prompt": "新闻文本是*ST大药表示，“所涉事项与公司无关，截至本公告披露日，公司未被相关机关要求协助调查，包含的情绪词典是nondisclosure：0.0，noncompliant：-0.5"}, "” 　　公告显示，杨君祥在留置期间暂时无法履行法定代表人、董事长、总经理的职责，董事会审议通过了在杨君祥留置期间，由副董事长尹翠仙代为履行公司法定代表人、董事长的职责，以及代为履行董事会相关委员会成员的职责": {"topic": null, "similarity": null, "prompt": "新闻文本是” 　　公告显示，杨君祥在留置期间暂时无法履行法定代表人、董事长、总经理的职责，董事会审议通过了在杨君祥留置期间，由副董事长尹翠仙代为履行公司法定代表人、董事长的职责，以及代为履行董事会相关委员会成员的职责，包含的情绪词典是company：0.0，enterprise：0.0"}, "此外，经杨君祥书面授权，留置期间由董事会秘书吴佩容代为履行总经理的职责": {"topic": null, "similarity": null, "prompt": "新闻文本是此外，经杨君祥书面授权，留置期间由董事会秘书吴佩容代为履行总经理的职责，包含的情绪词典是executors：0.0，executory：0.0"}, "*ST大药还表示，公司其他董事、监事和高级管理人员均正常履职，控制权未发生变化，董事会运作正常，生产经营管理情况正常，上述事项不会对正常生产经营产生重大影响": {"topic": null, "similarity": null, "prompt": "新闻文本是*ST大药还表示，公司其他董事、监事和高级管理人员均正常履职，控制权未发生变化，董事会运作正常，生产经营管理情况正常，上述事项不会对正常生产经营产生重大影响，包含的情绪词典是executrixes：0.0，stock：0.0"}, "图片来源：*ST大药公告截图　　*ST大药2024年半年报显示，杨君祥家族（杨君祥、杨清龙、尹翠仙）为实际控制人，分别直接持有23.31%、11.94%和3.06%的股份，合计持有38.31%的上市公司股份": {"topic": null, "similarity": null, "prompt": "新闻文本是图片来源：*ST大药公告截图　　*ST大药2024年半年报显示，杨君祥家族（杨君祥、杨清龙、尹翠仙）为实际控制人，分别直接持有23.31%、11.94%和3.06%的股份，合计持有38.31%的上市公司股份，包含的情绪词典是enterprise：0.0，stock：0.0"}, "公开信息显示，杨清龙为杨君祥之子，尹翠仙为杨君祥之妻": {"topic": null, "similarity": null, "prompt": "新闻文本是公开信息显示，杨清龙为杨君祥之子，尹翠仙为杨君祥之妻，包含的情绪词典是public：0.0，chinese：0.0"}, "值得一提的是，8月以来已有大胜达（603687.SH）、徕木股份（603633.SH）先后发布留置公告，上述消息发布后两家公司次日股价均以跌停收盘": {"topic": "金融", "similarity": 0.3826306462287903, "prompt": "新闻文本是值得一提的是，8月以来已有大胜达（603687.SH）、徕木股份（603633.SH）先后发布留置公告，上述消息发布后两家公司次日股价均以跌停收盘，包含的情绪词典是stock：0.0，stay：0.0"}, "（文章来源：21世纪经济报道）": {"topic": null, "similarity": null, "prompt": "新闻文本是（文章来源：21世纪经济报道），包含的情绪词典是economic：0.0，economy：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>{"央行：二季度末个人住房贷款余额37.79万亿元，同比下降2.1%": {"topic": "房地产", "similarity": 0.4318600594997406}, "中央汇金大幅加仓，继续增持头部宽基ETF": {"topic": "金融", "similarity": 0.37267881631851196}, "A股上市公司中期分红近5300亿元，创历史新高": {"topic": "金融", "similarity": 0.38382238149642944}, "广州：全市新房开始推行“买房即交房、交证”": {"topic": "房地产", "similarity": 0.41722941398620605}, "热点聚焦 　　国常会：研究推动保险业高质量发展的若干意见 　　8月30日召开的国务院常务会议，研究推动保险业高质量发展的若干意见，部署落实大食物观相关工作，审议通过《加快完善海河流域防洪体系实施方案》和《网络数据安全管理条例（草案）》，讨论《中华人民共和国海商法（修订草案）》": {"topic": "宏观经济", "similarity": 0.4165666699409485}, "会议指出，保险业在保障和改善民生、防灾减损、服务实体经济等方面具有重要作用": {"topic": "金融", "similarity": 0.37440118193626404}, "要夯实保险业高质量发展制度基础，牢固树立服务优先理念，充分发挥商业保险等市场机制作用，大力提升保险业保障能力和服务水平": {"topic": "金融", "similarity": 0.3921348452568054}, "要紧盯关键领域和薄弱环节加强监管，保障消费者合法权益，健全风险防范制度体系": {"topic": "消费", "similarity": 0.514423668384552}, "要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资": {"topic": "金融", "similarity": 0.40698006749153137}, "央行8月净买入国债1000亿元 　　中国人民银行8月30日首次发布国债买卖业务公告称，为贯彻落实中央金融工作会议相关要求，8月人民银行开展了公开市场国债买卖操作，向部分公开市场业务一级交易商买入短期限国债并卖出长期限国债，全月净买入债券面值为1000亿元": {"topic": "金融", "similarity": 0.4486016631126404}, "央行净买入1000亿元国债，实际是向公开市场投放了基础货币": {"topic": "金融", "similarity": 0.38340967893600464}, "”民生银行首席经济学家温彬对证券时报记者表示": {"topic": "金融", "similarity": 0.452503502368927}, "随着公开市场国债买卖操作正式纳入货币政策工具箱，金融资源的配置效率有望进一步提升": {"topic": "金融", "similarity": 0.39444005489349365}, "受访专家学者认为，央行通过增加国债的买卖规模和频率精准调控银行间流动性，并避免再贷款等工具大规模到期续作时的扰动": {"topic": "宏观经济", "similarity": 0.39031827449798584}, "央行：二季度末个人住房贷款余额37.79万亿元同比降2.1% 　　央行发布2024年二季度金融机构贷款投向统计报告，2024年二季度末，房地产开发贷款余额13.77万亿元，同比增长2.8%，增速比上年末高1.3个百分点，上半年增加6105亿元": {"topic": "房地产", "similarity": 0.5163979530334473}, "个人住房贷款余额37.79万亿元，同比下降2.1%": {"topic": "房地产", "similarity": 0.4126608669757843}, "2024年二季度末，人民币房地产贷款余额53.1万亿元，同比下降1%，增速比上年末高0.04个百分点": {"topic": "房地产", "similarity": 0.40994927287101746}, "财政部：将加大财政政策实施力度 　　财政部发布2024年上半年中国财政政策执行情况报告": {"topic": "宏观经济", "similarity": 0.4222736656665802}, "下一步，将加大财政政策实施力度": {"topic": "宏观经济", "similarity": 0.3707787096500397}, "统筹安排和用好超长期特别国债资金，通过增规模、降门槛、扩范围、简流程，优化设备更新支持方式": {"topic": "生产投资", "similarity": 0.37505272030830383}, "通过增强地方自主权、发挥地方创造力，支持地方提升消费品以旧换新能力": {"topic": "消费", "similarity": 0.40081530809402466}, "实施好汽车以旧换新补贴、新能源城市公交车及动力电池更新补贴等政策": {"topic": "宏观经济", "similarity": 0.39634886384010315}, "二是更好发挥政府投资带动放大效应": {"topic": "生产投资", "similarity": 0.40216588973999023}, "积极引导社会资本参与，着力提高投资综合效益": {"topic": "生产投资", "similarity": 0.4015890657901764}, "更好发挥关税等宏观调控职能，进一步优化调整进口税收政策": {"topic": "宏观经济", "similarity": 0.4632091522216797}, "四是切实加强与货币等其他政策协同": {"topic": "宏观经济", "similarity": 0.4144708812236786}, "综合运用政策性金融、贴息奖补、融资担保等政策工具，支持和撬动更多资金精准支持经济社会发展重点领域和薄弱环节": {"topic": "宏观经济", "similarity": 0.4633478820323944}, "财政部：建立全口径地方债务监测机制坚决遏制化债不实和新增隐性债务 　　财政部发布2024年上半年中国财政政策执行情况报告": {"topic": "宏观经济", "similarity": 0.46820539236068726}, "下一步，防范化解地方政府债务风险": {"topic": "房地产", "similarity": 0.3758170008659363}, "加强融资需求端和供给端管控，强化政府支出事项和政府投资项目管理，规范金融机构融资业务，阻断新增隐性债务路径": {"topic": "宏观经济", "similarity": 0.4341917634010315}, "建立全口径地方债务监测机制，加强跨部门数据信息共享应用，加大协同监管和追责问责力度，坚决遏制化债不实和新增隐性债务": {"topic": "房地产", "similarity": 0.4132222533226013}}</t>
+          <t>{"摘要 　　国常会：研究推动保险业高质量发展的若干意见": {"topic": null, "similarity": null, "prompt": "新闻文本是摘要 　　国常会：研究推动保险业高质量发展的若干意见，包含的情绪词典是consecutive：0.0，development：0.4"}, "央行8月净买入国债1000亿元": {"topic": null, "similarity": null, "prompt": "新闻文本是央行8月净买入国债1000亿元，包含的情绪词典是bank：0.0，financial：0.0"}, "央行：二季度末个人住房贷款余额37.79万亿元，同比下降2.1%": {"topic": "房地产", "similarity": 0.43185994029045105, "prompt": "新闻文本是央行：二季度末个人住房贷款余额37.79万亿元，同比下降2.1%，包含的情绪词典是bank：0.0，finance：0.0"}, "财政部：将加大财政政策实施力度": {"topic": null, "similarity": null, "prompt": "新闻文本是财政部：将加大财政政策实施力度，包含的情绪词典是finance：0.0，financial：0.0"}, "商务部等五部门联合出台《推动电动自行车以旧换新实施方案》": {"topic": null, "similarity": null, "prompt": "新闻文本是商务部等五部门联合出台《推动电动自行车以旧换新实施方案》，包含的情绪词典是vehicle：0.0，car：0.0"}, "中央汇金大幅加仓，继续增持头部宽基ETF": {"topic": "金融", "similarity": 0.3726786971092224, "prompt": "新闻文本是中央汇金大幅加仓，继续增持头部宽基ETF，包含的情绪词典是invest：0.3，stock：0.0"}, "A股上市公司中期分红近5300亿元，创历史新高": {"topic": "金融", "similarity": 0.38382217288017273, "prompt": "新闻文本是A股上市公司中期分红近5300亿元，创历史新高，包含的情绪词典是stock：0.0，profit：0.8"}, "广州：全市新房开始推行“买房即交房、交证”": {"topic": "房地产", "similarity": 0.4172292947769165, "prompt": "新闻文本是广州：全市新房开始推行“买房即交房、交证”，包含的情绪词典是house：0.0，household：0.0"}, "热点聚焦 　　国常会：研究推动保险业高质量发展的若干意见 　　8月30日召开的国务院常务会议，研究推动保险业高质量发展的若干意见，部署落实大食物观相关工作，审议通过《加快完善海河流域防洪体系实施方案》和《网络数据安全管理条例（草案）》，讨论《中华人民共和国海商法（修订草案）》": {"topic": "宏观经济", "similarity": 0.41656675934791565, "prompt": "新闻文本是热点聚焦 　　国常会：研究推动保险业高质量发展的若干意见 　　8月30日召开的国务院常务会议，研究推动保险业高质量发展的若干意见，部署落实大食物观相关工作，审议通过《加快完善海河流域防洪体系实施方案》和《网络数据安全管理条例（草案）》，讨论《中华人民共和国海商法（修订草案）》，包含的情绪词典是food：0.0，risk：-0.4"}, "会议指出，保险业在保障和改善民生、防灾减损、服务实体经济等方面具有重要作用": {"topic": "金融", "similarity": 0.3744010925292969, "prompt": "新闻文本是会议指出，保险业在保障和改善民生、防灾减损、服务实体经济等方面具有重要作用，包含的情绪词典是risk：-0.4，risks：-0.4"}, "要夯实保险业高质量发展制度基础，牢固树立服务优先理念，充分发挥商业保险等市场机制作用，大力提升保险业保障能力和服务水平": {"topic": "金融", "similarity": 0.39213472604751587, "prompt": "新闻文本是要夯实保险业高质量发展制度基础，牢固树立服务优先理念，充分发挥商业保险等市场机制作用，大力提升保险业保障能力和服务水平，包含的情绪词典是service：0.0，advancement：0.5"}, "要紧盯关键领域和薄弱环节加强监管，保障消费者合法权益，健全风险防范制度体系": {"topic": "消费", "similarity": 0.5144236087799072, "prompt": "新闻文本是要紧盯关键领域和薄弱环节加强监管，保障消费者合法权益，健全风险防范制度体系，包含的情绪词典是consumer：0.0，focus：0.0"}, "要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资": {"topic": "金融", "similarity": 0.4069799482822418, "prompt": "新闻文本是要培育壮大保险资金等耐心资本，打通制度障碍，完善考核评估机制，为资本市场和科技创新提供稳定的长期投资，包含的情绪词典是investment：0.4，invest：0.3"}, "央行8月净买入国债1000亿元 　　中国人民银行8月30日首次发布国债买卖业务公告称，为贯彻落实中央金融工作会议相关要求，8月人民银行开展了公开市场国债买卖操作，向部分公开市场业务一级交易商买入短期限国债并卖出长期限国债，全月净买入债券面值为1000亿元": {"topic": "金融", "similarity": 0.4486015737056732, "prompt": "新闻文本是央行8月净买入国债1000亿元 　　中国人民银行8月30日首次发布国债买卖业务公告称，为贯彻落实中央金融工作会议相关要求，8月人民银行开展了公开市场国债买卖操作，向部分公开市场业务一级交易商买入短期限国债并卖出长期限国债，全月净买入债券面值为1000亿元，包含的情绪词典是finance：0.0，financial：0.0"}, "央行净买入1000亿元国债，实际是向公开市场投放了基础货币": {"topic": "金融", "similarity": 0.38340964913368225, "prompt": "新闻文本是央行净买入1000亿元国债，实际是向公开市场投放了基础货币，包含的情绪词典是money：0.2，financial：0.0"}, "“这表明了央行支持性的货币政策立场，预示着后续流动性的合理充裕状态": {"topic": null, "similarity": null, "prompt": "新闻文本是“这表明了央行支持性的货币政策立场，预示着后续流动性的合理充裕状态，包含的情绪词典是bank：0.0，possibility：0.1"}, "”民生银行首席经济学家温彬对证券时报记者表示": {"topic": "金融", "similarity": 0.452503502368927, "prompt": "新闻文本是”民生银行首席经济学家温彬对证券时报记者表示，包含的情绪词典是bank：0.0，economic：0.0"}, "随着公开市场国债买卖操作正式纳入货币政策工具箱，金融资源的配置效率有望进一步提升": {"topic": "金融", "similarity": 0.3944399952888489, "prompt": "新闻文本是随着公开市场国债买卖操作正式纳入货币政策工具箱，金融资源的配置效率有望进一步提升，包含的情绪词典是finance：0.0，financial：0.0"}, "受访专家学者认为，央行通过增加国债的买卖规模和频率精准调控银行间流动性，并避免再贷款等工具大规模到期续作时的扰动": {"topic": "宏观经济", "similarity": 0.39031827449798584, "prompt": "新闻文本是受访专家学者认为，央行通过增加国债的买卖规模和频率精准调控银行间流动性，并避免再贷款等工具大规模到期续作时的扰动，包含的情绪词典是bank：0.0，finance：0.0"}, "央行：二季度末个人住房贷款余额37.79万亿元同比降2.1% 　　央行发布2024年二季度金融机构贷款投向统计报告，2024年二季度末，房地产开发贷款余额13.77万亿元，同比增长2.8%，增速比上年末高1.3个百分点，上半年增加6105亿元": {"topic": "房地产", "similarity": 0.5163979530334473, "prompt": "新闻文本是央行：二季度末个人住房贷款余额37.79万亿元同比降2.1% 　　央行发布2024年二季度金融机构贷款投向统计报告，2024年二季度末，房地产开发贷款余额13.77万亿元，同比增长2.8%，增速比上年末高1.3个百分点，上半年增加6105亿元，包含的情绪词典是bank：0.0，finance：0.0"}, "个人住房贷款余额37.79万亿元，同比下降2.1%": {"topic": "房地产", "similarity": 0.4126608967781067, "prompt": "新闻文本是个人住房贷款余额37.79万亿元，同比下降2.1%，包含的情绪词典是finance：0.0，house：0.0"}, "2024年二季度末，人民币房地产贷款余额53.1万亿元，同比下降1%，增速比上年末高0.04个百分点": {"topic": "房地产", "similarity": 0.4099491834640503, "prompt": "新闻文本是2024年二季度末，人民币房地产贷款余额53.1万亿元，同比下降1%，增速比上年末高0.04个百分点，包含的情绪词典是recession：-0.95，investment：0.4"}, "上半年增加1976亿元，同比多增427亿元": {"topic": null, "similarity": null, "prompt": "新闻文本是上半年增加1976亿元，同比多增427亿元，包含的情绪词典是financial：0.0，money：0.2"}, "财政部：将加大财政政策实施力度 　　财政部发布2024年上半年中国财政政策执行情况报告": {"topic": "宏观经济", "similarity": 0.422273725271225, "prompt": "新闻文本是财政部：将加大财政政策实施力度 　　财政部发布2024年上半年中国财政政策执行情况报告，包含的情绪词典是finance：0.0，financial：0.0"}, "下一步，将加大财政政策实施力度": {"topic": "宏观经济", "similarity": 0.3707786798477173, "prompt": "新闻文本是下一步，将加大财政政策实施力度，包含的情绪词典是financial：0.0，policy：0.0"}, "一是加力支持“两新”工作": {"topic": null, "similarity": null, "prompt": "新闻文本是一是加力支持“两新”工作，包含的情绪词典是new：0.0，innovation：0.7"}, "统筹安排和用好超长期特别国债资金，通过增规模、降门槛、扩范围、简流程，优化设备更新支持方式": {"topic": "生产投资", "similarity": 0.3750527799129486, "prompt": "新闻文本是统筹安排和用好超长期特别国债资金，通过增规模、降门槛、扩范围、简流程，优化设备更新支持方式，包含的情绪词典是improvement：0.6，update：0.0"}, "通过增强地方自主权、发挥地方创造力，支持地方提升消费品以旧换新能力": {"topic": "消费", "similarity": 0.40081533789634705, "prompt": "新闻文本是通过增强地方自主权、发挥地方创造力，支持地方提升消费品以旧换新能力，包含的情绪词典是improvement：0.6，local：0.0"}, "实施好汽车以旧换新补贴、新能源城市公交车及动力电池更新补贴等政策": {"topic": "宏观经济", "similarity": 0.396348774433136, "prompt": "新闻文本是实施好汽车以旧换新补贴、新能源城市公交车及动力电池更新补贴等政策，包含的情绪词典是vehicle：0.0，car：0.0"}, "二是更好发挥政府投资带动放大效应": {"topic": "生产投资", "similarity": 0.402165949344635, "prompt": "新闻文本是二是更好发挥政府投资带动放大效应，包含的情绪词典是investment：0.4，invest：0.3"}, "发行并用好超长期特别国债，支持“两重”建设": {"topic": null, "similarity": null, "prompt": "新闻文本是发行并用好超长期特别国债，支持“两重”建设，包含的情绪词典是recessionary：-0.8，money：0.2"}, "加快地方政府专项债券发行使用，形成更多实物工作量": {"topic": null, "similarity": null, "prompt": "新闻文本是加快地方政府专项债券发行使用，形成更多实物工作量，包含的情绪词典是proactively：0.5，work：0.01"}, "积极引导社会资本参与，着力提高投资综合效益": {"topic": "生产投资", "similarity": 0.40158912539482117, "prompt": "新闻文本是积极引导社会资本参与，着力提高投资综合效益，包含的情绪词典是capital：0.1，invest：0.3"}, "三是持续优化和落实好税费优惠政策": {"topic": null, "similarity": null, "prompt": "新闻文本是三是持续优化和落实好税费优惠政策，包含的情绪词典是improvement：0.6，improving：0.5"}, "更好发挥关税等宏观调控职能，进一步优化调整进口税收政策": {"topic": "宏观经济", "similarity": 0.46320897340774536, "prompt": "新闻文本是更好发挥关税等宏观调控职能，进一步优化调整进口税收政策，包含的情绪词典是improving：0.5，improvement：0.6"}, "四是切实加强与货币等其他政策协同": {"topic": "宏观经济", "similarity": 0.4144708812236786, "prompt": "新闻文本是四是切实加强与货币等其他政策协同，包含的情绪词典是policy：0.0，financial：0.0"}, "综合运用政策性金融、贴息奖补、融资担保等政策工具，支持和撬动更多资金精准支持经济社会发展重点领域和薄弱环节": {"topic": "宏观经济", "similarity": 0.4633479416370392, "prompt": "新闻文本是综合运用政策性金融、贴息奖补、融资担保等政策工具，支持和撬动更多资金精准支持经济社会发展重点领域和薄弱环节，包含的情绪词典是finance：0.0，contention：-0.3"}, "五是密切跟踪预算执行和政策落实情况": {"topic": null, "similarity": null, "prompt": "新闻文本是五是密切跟踪预算执行和政策落实情况，包含的情绪词典是policy：0.0，follow：0.0"}, "财政部：建立全口径地方债务监测机制坚决遏制化债不实和新增隐性债务 　　财政部发布2024年上半年中国财政政策执行情况报告": {"topic": "宏观经济", "similarity": 0.4682054817676544, "prompt": "新闻文本是财政部：建立全口径地方债务监测机制坚决遏制化债不实和新增隐性债务 　　财政部发布2024年上半年中国财政政策执行情况报告，包含的情绪词典是finance：0.0，government：0.0"}, "下一步，防范化解地方政府债务风险": {"topic": "房地产", "similarity": 0.37581709027290344, "prompt": "新闻文本是下一步，防范化解地方政府债务风险，包含的情绪词典是risks：-0.4，risk：-0.4"}, "统筹好风险化解和稳定发展，进一步落实一揽子化债方案，省负总责、市县尽全力化债，逐步降低债务风险水平": {"topic": null, "similarity": null, "prompt": "新闻文本是统筹好风险化解和稳定发展，进一步落实一揽子化债方案，省负总责、市县尽全力化债，逐步降低债务风险水平，包含的情绪词典是risk：-0.4，risks：-0.4"}, "加强融资需求端和供给端管控，强化政府支出事项和政府投资项目管理，规范金融机构融资业务，阻断新增隐性债务路径": {"topic": "宏观经济", "similarity": 0.4341917335987091, "prompt": "新闻文本是加强融资需求端和供给端管控，强化政府支出事项和政府投资项目管理，规范金融机构融资业务，阻断新增隐性债务路径，包含的情绪词典是finance：0.0，investment：0.4"}, "建立全口径地方债务监测机制，加强跨部门数据信息共享应用，加大协同监管和追责问责力度，坚决遏制化债不实和新增隐性债务": {"topic": "房地产", "similarity": 0.41322219371795654, "prompt": "新闻文本是建立全口径地方债务监测机制，加强跨部门数据信息共享应用，加大协同监管和追责问责力度，坚决遏制化债不实和新增隐性债务，包含的情绪词典是finance：0.0，financial：0.0"}, "分类推进融资平台公司改革转型，加快压降平台数量和隐性债务规模": {"topic": null, "similarity": null, "prompt": "新闻文本是分类推进融资平台公司改革转型，加快压降平台数量和隐性债务规模，包含的情绪词典是company：0.0，finance：0.0"}, "完善专项债券管理制度，强化项目资产管理、收入归集，确保按时偿还、不出风险": {"topic": null, "similarity": null, "prompt": "新闻文本是完善专项债券管理制度，强化项目资产管理、收入归集，确保按时偿还、不出风险，包含的情绪词典是investment：0.4，finance：0.0"}, "五部门联合出台《推动电动自行车以旧换新实施方案》 　　8月30日，商务部、工业和信息化部、生态环境部、市场监管总局、国家消防救援局等五部门印发《推动电动自行车以旧换新实施方案》，这是我国首次出台电动自行车以旧换新政策": {"topic": null, "similarity": null, "prompt": "新闻文本是五部门联合出台《推动电动自行车以旧换新实施方案》 　　8月30日，商务部、工业和信息化部、生态环境部、市场监管总局、国家消防救援局等五部门印发《推动电动自行车以旧换新实施方案》，这是我国首次出台电动自行车以旧换新政策，包含的情绪词典是vehicle：0.0，automobile：0.0"}, "《实施方案》指出，各地要统筹用好加力支持消费品以旧换新相关资金，结合实际制定电动自行车以旧换新实施方案，对交回个人名下老旧电动自行车并换购电动自行车新车的消费者予以补贴，鼓励享受补": {"topic": null, "similarity": null, "prompt": "新闻文本是《实施方案》指出，各地要统筹用好加力支持消费品以旧换新相关资金，结合实际制定电动自行车以旧换新实施方案，对交回个人名下老旧电动自行车并换购电动自行车新车的消费者予以补贴，鼓励享受补，包含的情绪词典是electrical：0.0，update：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>{"据目前安排，若无变化本周（9月2日到6日）共有3只新股申购": {"topic": "金融", "similarity": 0.4111081659793854}, "其中上证主板1只，创业板1只，北交所1只": {"topic": "金融", "similarity": 0.4801737070083618}, "9月6日启动打新的上证主板众鑫股份是国内规模较大的可降解纸浆模塑餐饮具制造商，已形成了年产12.37万吨的自然降解植物纤维模塑产品的生产能力": {"topic": "金融", "similarity": 0.3814663887023926}, "众鑫股份产品广泛应用于餐饮、快消、医疗、工业等领域，以外销为主，但内销呈快速增长趋势": {"topic": "生产投资", "similarity": 0.4091598391532898}, "2股已披露发行价 　　截至发稿，本周网上发行的2只新股已披露发行价：创业板新股慧翰股份发行价为39.84元，发行市盈率22.57倍，行业最近一个月平均动态市盈率29.08倍": {"topic": "金融", "similarity": 0.43214845657348633}, "本次IPO，慧翰股份募集总额6.99亿元，用于研发中心建设项目、智能汽车安全系统和5G车联网TBOX研发及产业化项目": {"topic": "金融", "similarity": 0.3780222237110138}, "众鑫股份在浙江金华、广西来宾等地拥有多个生产基地，已形成年产10.29万吨的自然降解植物纤维模塑产品的生产能力，产品销往80多个国家和地区": {"topic": "生产投资", "similarity": 0.3873157501220703}, "业绩方面，2020至2022年，众鑫股份实现营业收入5.78亿元、9.1亿元及13.16亿元，年均复合增长率为50.89%": {"topic": "金融", "similarity": 0.3755682706832886}, "本次IPO，众鑫股份拟募集15.38亿元投资建设2个年产10万吨甘蔗渣可降解环保餐具项目及研发中心设施等": {"topic": "生产投资", "similarity": 0.39538872241973877}, "8月新股首日平均涨幅达152% 　　回顾8月至今的新股表现，投资情绪持续回暖": {"topic": "金融", "similarity": 0.44412147998809814}, "8月登陆A股的9只新股无一首日破发，其中6只新股首日涨幅更实现翻倍，占比达67%": {"topic": "金融", "similarity": 0.4047330915927887}, "按收盘价计算，8月至今上市的9只新股首日平均涨幅达到152.47%": {"topic": "金融", "similarity": 0.42442017793655396}, "其中，8月16日珂玛科技正式登陆创业板挂牌上市": {"topic": "金融", "similarity": 0.37283191084861755}, "放在全年观察，珂玛科技首日涨幅也仅次于汇成真空，排名第二": {"topic": "通货膨胀", "similarity": 0.395606130361557}, "根据弗若斯特沙利文数据，2021年珂玛科技占中国内地国产半导体设备的先进结构陶瓷采购总规模的约14%，占中国内地国产半导体设备的内地本土先进结构陶瓷供应商供应总规模的约72%": {"topic": "生产投资", "similarity": 0.38025230169296265}, "同时，珂玛科技也是目前国内少数有多种陶瓷材料和产品通过国际头部半导体设备厂商A公司认证的先进结构陶瓷企业之一": {"topic": "生产投资", "similarity": 0.3723471164703369}, "打新日历 　　9月2日 　　慧翰股份（301600）是一家致力于为智能汽车及产业物联网客户提供智能网联解决方案的科技服务商，主要从事车联网智能终端、物联网智能模组的研发、生产和销售，同时为客户提供软件和技术服务": {"topic": "金融", "similarity": 0.3937978446483612}}</t>
+          <t>{"据目前安排，若无变化本周（9月2日到6日）共有3只新股申购": {"topic": "金融", "similarity": 0.41110801696777344, "prompt": "新闻文本是据目前安排，若无变化本周（9月2日到6日）共有3只新股申购，包含的情绪词典是stock：0.0，stockpile：0.1"}, "其中上证主板1只，创业板1只，北交所1只": {"topic": "金融", "similarity": 0.48017358779907227, "prompt": "新闻文本是其中上证主板1只，创业板1只，北交所1只，包含的情绪词典是board：0.0，stock：0.0"}, "9月6日启动打新的上证主板众鑫股份是国内规模较大的可降解纸浆模塑餐饮具制造商，已形成了年产12.37万吨的自然降解植物纤维模塑产品的生产能力": {"topic": "金融", "similarity": 0.38146650791168213, "prompt": "新闻文本是9月6日启动打新的上证主板众鑫股份是国内规模较大的可降解纸浆模塑餐饮具制造商，已形成了年产12.37万吨的自然降解植物纤维模塑产品的生产能力，包含的情绪词典是enterprise：0.0，industry：0.0"}, "2022年，众鑫股份在全球纸浆模塑餐饮具领域的市场占有率约16%，产量占全国纸浆模塑餐饮具产量的20%": {"topic": null, "similarity": null, "prompt": "新闻文本是2022年，众鑫股份在全球纸浆模塑餐饮具领域的市场占有率约16%，产量占全国纸浆模塑餐饮具产量的20%，包含的情绪词典是commercial：0.0，industrial：0.0"}, "众鑫股份产品广泛应用于餐饮、快消、医疗、工业等领域，以外销为主，但内销呈快速增长趋势": {"topic": "生产投资", "similarity": 0.409159779548645, "prompt": "新闻文本是众鑫股份产品广泛应用于餐饮、快消、医疗、工业等领域，以外销为主，但内销呈快速增长趋势，包含的情绪词典是company：0.0，industry：0.0"}, "2股已披露发行价 　　截至发稿，本周网上发行的2只新股已披露发行价：创业板新股慧翰股份发行价为39.84元，发行市盈率22.57倍，行业最近一个月平均动态市盈率29.08倍": {"topic": "金融", "similarity": 0.43214839696884155, "prompt": "新闻文本是2股已披露发行价 　　截至发稿，本周网上发行的2只新股已披露发行价：创业板新股慧翰股份发行价为39.84元，发行市盈率22.57倍，行业最近一个月平均动态市盈率29.08倍，包含的情绪词典是stock：0.0，price：0.0"}, "北交所新股中草香料发行价为7.5元，发行市盈率15.37倍，行业最近一个月平均动态市盈率18.72倍": {"topic": null, "similarity": null, "prompt": "新闻文本是北交所新股中草香料发行价为7.5元，发行市盈率15.37倍，行业最近一个月平均动态市盈率18.72倍，包含的情绪词典是stock：0.0，price：0.0"}, "慧翰股份主要从事车联网智能终端、物联网智能模组的研发、生产和销售，同时为客户提供软件和技术服务": {"topic": null, "similarity": null, "prompt": "新闻文本是慧翰股份主要从事车联网智能终端、物联网智能模组的研发、生产和销售，同时为客户提供软件和技术服务，包含的情绪词典是company：0.0，automobile：0.0"}, "在车联网领域，慧翰股份为上汽集团、奇瑞汽车、吉利汽车、比亚迪、宁德时代、德赛西威等智能汽车产业领先的整车厂商及其一级供应商提供车联网智能终端、物联网智能模组和解决方案": {"topic": null, "similarity": null, "prompt": "新闻文本是在车联网领域，慧翰股份为上汽集团、奇瑞汽车、吉利汽车、比亚迪、宁德时代、德赛西威等智能汽车产业领先的整车厂商及其一级供应商提供车联网智能终端、物联网智能模组和解决方案，包含的情绪词典是automobile：0.0，automotive：0.0"}, "在其他产业物联网领域，慧翰股份为Microchip、Sierra和Cerence等全球知名物联网解决方案供应商提供智能模组及智能单元": {"topic": null, "similarity": null, "prompt": "新闻文本是在其他产业物联网领域，慧翰股份为Microchip、Sierra和Cerence等全球知名物联网解决方案供应商提供智能模组及智能单元，包含的情绪词典是industry：0.0，enterprise：0.0"}, "慧翰股份近年来营收和利润均高速增长": {"topic": null, "similarity": null, "prompt": "新闻文本是慧翰股份近年来营收和利润均高速增长，包含的情绪词典是growth：0.7，profitability：0.6"}, "业绩方面，2021年至2023年，公司实现营收分别为4.2亿元、5.8亿元和8.1亿元，复合增长率为38.85%": {"topic": null, "similarity": null, "prompt": "新闻文本是业绩方面，2021年至2023年，公司实现营收分别为4.2亿元、5.8亿元和8.1亿元，复合增长率为38.85%，包含的情绪词典是profitability：0.6，profit：0.8"}, "扣非净利润分别为5838.27万元、8333.04万元和12382.96万元，复合增长率为45.64%": {"topic": null, "similarity": null, "prompt": "新闻文本是扣非净利润分别为5838.27万元、8333.04万元和12382.96万元，复合增长率为45.64%，包含的情绪词典是profitability：0.6，profit：0.8"}, "2024年1至6月，慧翰股份实现营收4.3亿元，同比增长31.13%": {"topic": null, "similarity": null, "prompt": "新闻文本是2024年1至6月，慧翰股份实现营收4.3亿元，同比增长31.13%，包含的情绪词典是profitability：0.6，profit：0.8"}, "扣非净利润7158.34万元，同比增长38.51%": {"topic": null, "similarity": null, "prompt": "新闻文本是扣非净利润7158.34万元，同比增长38.51%，包含的情绪词典是profitability：0.6，profitable：0.8"}, "公司车联网TBOX、eCall终端和智能模组已经具备领先的市场地位和产品竞争力": {"topic": null, "similarity": null, "prompt": "新闻文本是公司车联网TBOX、eCall终端和智能模组已经具备领先的市场地位和产品竞争力，包含的情绪词典是company：0.0，enterprise：0.0"}, "本次IPO，慧翰股份募集总额6.99亿元，用于研发中心建设项目、智能汽车安全系统和5G车联网TBOX研发及产业化项目": {"topic": "金融", "similarity": 0.3780221939086914, "prompt": "新闻文本是本次IPO，慧翰股份募集总额6.99亿元，用于研发中心建设项目、智能汽车安全系统和5G车联网TBOX研发及产业化项目，包含的情绪词典是investment：0.4，automobile：0.0"}, "本周启动打新的众鑫股份是全球纸浆模塑环保餐具龙头企业": {"topic": null, "similarity": null, "prompt": "新闻文本是本周启动打新的众鑫股份是全球纸浆模塑环保餐具龙头企业，包含的情绪词典是company：0.0，industry：0.0"}, "众鑫股份在浙江金华、广西来宾等地拥有多个生产基地，已形成年产10.29万吨的自然降解植物纤维模塑产品的生产能力，产品销往80多个国家和地区": {"topic": "生产投资", "similarity": 0.3873157203197479, "prompt": "新闻文本是众鑫股份在浙江金华、广西来宾等地拥有多个生产基地，已形成年产10.29万吨的自然降解植物纤维模塑产品的生产能力，产品销往80多个国家和地区，包含的情绪词典是enterprise：0.0，industrial：0.0"}, "业绩方面，2020至2022年，众鑫股份实现营业收入5.78亿元、9.1亿元及13.16亿元，年均复合增长率为50.89%": {"topic": "金融", "similarity": 0.3755681812763214, "prompt": "新闻文本是业绩方面，2020至2022年，众鑫股份实现营业收入5.78亿元、9.1亿元及13.16亿元，年均复合增长率为50.89%，包含的情绪词典是profit：0.8，company：0.0"}, "扣非净利润7024.68万元、1.46亿元、2.06亿元，年均复合增长率为71.25%": {"topic": null, "similarity": null, "prompt": "新闻文本是扣非净利润7024.68万元、1.46亿元、2.06亿元，年均复合增长率为71.25%，包含的情绪词典是profit：0.8，profitability：0.6"}, "2023年上半年，众鑫股份实现营业收入6.05亿元，扣非净利润9509.19万元": {"topic": null, "similarity": null, "prompt": "新闻文本是2023年上半年，众鑫股份实现营业收入6.05亿元，扣非净利润9509.19万元，包含的情绪词典是profitability：0.6，profitable：0.8"}, "本次IPO，众鑫股份拟募集15.38亿元投资建设2个年产10万吨甘蔗渣可降解环保餐具项目及研发中心设施等": {"topic": "生产投资", "similarity": 0.3953888416290283, "prompt": "新闻文本是本次IPO，众鑫股份拟募集15.38亿元投资建设2个年产10万吨甘蔗渣可降解环保餐具项目及研发中心设施等，包含的情绪词典是investment：0.4，invest：0.3"}, "8月新股首日平均涨幅达152% 　　回顾8月至今的新股表现，投资情绪持续回暖": {"topic": "金融", "similarity": 0.44412142038345337, "prompt": "新闻文本是8月新股首日平均涨幅达152% 　　回顾8月至今的新股表现，投资情绪持续回暖，包含的情绪词典是stock：0.0，invest：0.3"}, "8月登陆A股的9只新股无一首日破发，其中6只新股首日涨幅更实现翻倍，占比达67%": {"topic": "金融", "similarity": 0.40473297238349915, "prompt": "新闻文本是8月登陆A股的9只新股无一首日破发，其中6只新股首日涨幅更实现翻倍，占比达67%，包含的情绪词典是stock：0.0，innovate：0.6"}, "按收盘价计算，8月至今上市的9只新股首日平均涨幅达到152.47%": {"topic": "金融", "similarity": 0.4244200587272644, "prompt": "新闻文本是按收盘价计算，8月至今上市的9只新股首日平均涨幅达到152.47%，包含的情绪词典是stock：0.0，price：0.0"}, "其中，8月16日珂玛科技正式登陆创业板挂牌上市": {"topic": "金融", "similarity": 0.3728318214416504, "prompt": "新闻文本是其中，8月16日珂玛科技正式登陆创业板挂牌上市，包含的情绪词典是tech：0.0，stock：0.0"}, "珂玛科技发行价8元/股，开盘价35.33元/股，当日涨幅高达368.25%，成为整个8月首日涨幅最高的新股": {"topic": null, "similarity": null, "prompt": "新闻文本是珂玛科技发行价8元/股，开盘价35.33元/股，当日涨幅高达368.25%，成为整个8月首日涨幅最高的新股，包含的情绪词典是highest：0.7，stock：0.0"}, "放在全年观察，珂玛科技首日涨幅也仅次于汇成真空，排名第二": {"topic": "通货膨胀", "similarity": 0.3956059217453003, "prompt": "新闻文本是放在全年观察，珂玛科技首日涨幅也仅次于汇成真空，排名第二，包含的情绪词典是yearly：0.0，tech：0.0"}, "珂玛科技位于苏州高新区，是国内本土半导体领域先进陶瓷材料及零部件的头部企业，获评国家高新技术企业及国家级专精特新“小巨人”企业等资质": {"topic": null, "similarity": null, "prompt": "新闻文本是珂玛科技位于苏州高新区，是国内本土半导体领域先进陶瓷材料及零部件的头部企业，获评国家高新技术企业及国家级专精特新“小巨人”企业等资质，包含的情绪词典是enterprise：0.0，industry：0.0"}, "根据弗若斯特沙利文数据，2021年珂玛科技占中国内地国产半导体设备的先进结构陶瓷采购总规模的约14%，占中国内地国产半导体设备的内地本土先进结构陶瓷供应商供应总规模的约72%": {"topic": "生产投资", "similarity": 0.3802524209022522, "prompt": "新闻文本是根据弗若斯特沙利文数据，2021年珂玛科技占中国内地国产半导体设备的先进结构陶瓷采购总规模的约14%，占中国内地国产半导体设备的内地本土先进结构陶瓷供应商供应总规模的约72%，包含的情绪词典是industry：0.0，tech：0.0"}, "同时，珂玛科技也是目前国内少数有多种陶瓷材料和产品通过国际头部半导体设备厂商A公司认证的先进结构陶瓷企业之一": {"topic": "生产投资", "similarity": 0.37234729528427124, "prompt": "新闻文本是同时，珂玛科技也是目前国内少数有多种陶瓷材料和产品通过国际头部半导体设备厂商A公司认证的先进结构陶瓷企业之一，包含的情绪词典是enterprise：0.0，industry：0.0"}, "打新日历 　　9月2日 　　慧翰股份（301600）是一家致力于为智能汽车及产业物联网客户提供智能网联解决方案的科技服务商，主要从事车联网智能终端、物联网智能模组的研发、生产和销售，同时为客户提供软件和技术服务": {"topic": "金融", "similarity": 0.39379775524139404, "prompt": "新闻文本是打新日历 　　9月2日 　　慧翰股份（301600）是一家致力于为智能汽车及产业物联网客户提供智能网联解决方案的科技服务商，主要从事车联网智能终端、物联网智能模组的研发、生产和销售，同时为客户提供软件和技术服务，包含的情绪词典是automobile：0.0，stock：0.0"}, "9月3日 　　中草香料（920016）是一家综合性香料香精制造企业，主营业务为天然香料、合成香料、植物精油、电子烟油和电子烟套装的研究开发、生产和销售": {"topic": null, "similarity": null, "prompt": "新闻文本是9月3日 　　中草香料（920016）是一家综合性香料香精制造企业，主营业务为天然香料、合成香料、植物精油、电子烟油和电子烟套装的研究开发、生产和销售，包含的情绪词典是enterprise：0.0，oil：0.0"}, "公司主要下游客户为香精调配企业，下游客户通过向公司采购天然香料、合成香料等来调配添加剂，并广泛应用于食品、日化、医药、烟草和化妆品等行业": {"topic": null, "similarity": null, "prompt": "新闻文本是公司主要下游客户为香精调配企业，下游客户通过向公司采购天然香料、合成香料等来调配添加剂，并广泛应用于食品、日化、医药、烟草和化妆品等行业，包含的情绪词典是company：0.0，enterprise：0.0"}, "9月6日 　　众鑫股份（603091）是一家专业从事自然降解植物纤维模塑产品的研发、生产和销售的高新技术企业": {"topic": null, "similarity": null, "prompt": "新闻文本是9月6日 　　众鑫股份（603091）是一家专业从事自然降解植物纤维模塑产品的研发、生产和销售的高新技术企业，包含的情绪词典是model：0.0，company：0.0"}, "公司产品主要利用蔗渣浆、竹浆等天然植物纤维材料，通过模具塑造成型，实现类似塑料产品吸塑、注塑工艺的造型效果，是塑料制品的良好替代，广泛应": {"topic": null, "similarity": null, "prompt": "新闻文本是公司产品主要利用蔗渣浆、竹浆等天然植物纤维材料，通过模具塑造成型，实现类似塑料产品吸塑、注塑工艺的造型效果，是塑料制品的良好替代，广泛应，包含的情绪词典是productive：0.7，industrial：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，中信建投研报指出，2024年上半年，根据样本数据，医疗器械板块收入同比增长1%，扣非归母净利润同比增长3%": {"topic": "金融", "similarity": 0.3932090401649475}, "去年下半年至今，医疗板块大幅调整，主要与医疗合规要求提升和医改政策背景下，不少上市公司的业绩缺乏确定性有关": {"topic": "金融", "similarity": 0.4367212653160095}, "展望三季度和四季度，市场对于医疗合规要求提升、飞检等医疗政策对行业的影响已有预期，近期不少个股的半年报业绩已落地、全年业绩预期将更加明朗": {"topic": "金融", "similarity": 0.41751521825790405}, "有国产替代和新品放量、出海业务快速发展逻辑的公司，有望在行业低基数背景下实现同比高增长、环比也有望改善，建议关注医疗器械行业的投资机会，重点把握业绩确定性强的方向及个股：集采逐步出清的院内器械、受医疗政策影响小的院外或海外器械、长期看好的器械龙头股价调整后的加仓机会": {"topic": "生产投资", "similarity": 0.44108492136001587}}</t>
+          <t>{"证券时报网讯，中信建投研报指出，2024年上半年，根据样本数据，医疗器械板块收入同比增长1%，扣非归母净利润同比增长3%": {"topic": "金融", "similarity": 0.39320898056030273, "prompt": "新闻文本是证券时报网讯，中信建投研报指出，2024年上半年，根据样本数据，医疗器械板块收入同比增长1%，扣非归母净利润同比增长3%，包含的情绪词典是industry：0.0，stock：0.0"}, "去年下半年至今，医疗板块大幅调整，主要与医疗合规要求提升和医改政策背景下，不少上市公司的业绩缺乏确定性有关": {"topic": "金融", "similarity": 0.43672123551368713, "prompt": "新闻文本是去年下半年至今，医疗板块大幅调整，主要与医疗合规要求提升和医改政策背景下，不少上市公司的业绩缺乏确定性有关，包含的情绪词典是stock：0.0，market：0.0"}, "展望三季度和四季度，市场对于医疗合规要求提升、飞检等医疗政策对行业的影响已有预期，近期不少个股的半年报业绩已落地、全年业绩预期将更加明朗": {"topic": "金融", "similarity": 0.4175150990486145, "prompt": "新闻文本是展望三季度和四季度，市场对于医疗合规要求提升、飞检等医疗政策对行业的影响已有预期，近期不少个股的半年报业绩已落地、全年业绩预期将更加明朗，包含的情绪词典是advancement：0.5，advance：0.6"}, "有国产替代和新品放量、出海业务快速发展逻辑的公司，有望在行业低基数背景下实现同比高增长、环比也有望改善，建议关注医疗器械行业的投资机会，重点把握业绩确定性强的方向及个股：集采逐步出清的院内器械、受医疗政策影响小的院外或海外器械、长期看好的器械龙头股价调整后的加仓机会": {"topic": "生产投资", "similarity": 0.44108492136001587, "prompt": "新闻文本是有国产替代和新品放量、出海业务快速发展逻辑的公司，有望在行业低基数背景下实现同比高增长、环比也有望改善，建议关注医疗器械行业的投资机会，重点把握业绩确定性强的方向及个股：集采逐步出清的院内器械、受医疗政策影响小的院外或海外器械、长期看好的器械龙头股价调整后的加仓机会，包含的情绪词典是stockpile：0.1，industry：0.0"}, "（文章来源：证券时报网）": {"topic": null, "similarity": null, "prompt": "新闻文本是（文章来源：证券时报网），包含的情绪词典是stock：0.0，finance：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -800,7 +800,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，证券时报·数据宝统计显示，社保基金最新出现在605只个股前十大流通股东名单中，合计持股量115.31亿股，期末持股市值合计1681.08亿元": {"topic": "金融", "similarity": 0.43087100982666016}, "持股变动显示，不变158只，减持162只，新进116只，增持169只": {"topic": "金融", "similarity": 0.4291473627090454}, "社保基金重仓股中，从前十大流通股东名单中社保基金家数来看，社保基金家数最多的是太阳纸业，共有5家社保基金出现在前十大流通股东名单中，即社保基金一零三组合、社保基金16042组合、社保基金一零九组合、社保基金16041组合、社保基金16012组合，分别位列公司第三大、第五大、第六大、第八大、第十大流通股东，持股量合计为1.73亿股，占流通股比例为6.26%": {"topic": "金融", "similarity": 0.4020301103591919}, "从持股比例看，社保基金持有比例最多的是英科再生，持股量占流通股比例为11.69%，其次是比音勒芬，社保基金持股比例为10.08%，持股比例居前的还有常熟银行、浙江荣泰、云路股份等": {"topic": "金融", "similarity": 0.38363683223724365}, "持股数量方面，社保基金持股数量在1亿股以上的共有16只，社保基金持股量最多的是常熟银行，共持有2.90亿股，分众传媒、广汇能源等紧随其后，持股量分别为2.65亿股、2.14亿股": {"topic": "金融", "similarity": 0.4685646891593933}}</t>
+          <t>{"证券时报网讯，证券时报·数据宝统计显示，社保基金最新出现在605只个股前十大流通股东名单中，合计持股量115.31亿股，期末持股市值合计1681.08亿元": {"topic": "金融", "similarity": 0.4308708906173706, "prompt": "新闻文本是证券时报网讯，证券时报·数据宝统计显示，社保基金最新出现在605只个股前十大流通股东名单中，合计持股量115.31亿股，期末持股市值合计1681.08亿元，包含的情绪词典是stock：0.0，financial：0.0"}, "持股变动显示，不变158只，减持162只，新进116只，增持169只": {"topic": "金融", "similarity": 0.42914730310440063, "prompt": "新闻文本是持股变动显示，不变158只，减持162只，新进116只，增持169只，包含的情绪词典是stock：0.0，investor：0.4"}, "社保基金重仓股中，从前十大流通股东名单中社保基金家数来看，社保基金家数最多的是太阳纸业，共有5家社保基金出现在前十大流通股东名单中，即社保基金一零三组合、社保基金16042组合、社保基金一零九组合、社保基金16041组合、社保基金16012组合，分别位列公司第三大、第五大、第六大、第八大、第十大流通股东，持股量合计为1.73亿股，占流通股比例为6.26%": {"topic": "金融", "similarity": 0.4020300507545471, "prompt": "新闻文本是社保基金重仓股中，从前十大流通股东名单中社保基金家数来看，社保基金家数最多的是太阳纸业，共有5家社保基金出现在前十大流通股东名单中，即社保基金一零三组合、社保基金16042组合、社保基金一零九组合、社保基金16041组合、社保基金16012组合，分别位列公司第三大、第五大、第六大、第八大、第十大流通股东，持股量合计为1.73亿股，占流通股比例为6.26%，包含的情绪词典是financial：0.0，stockpile：0.1"}, "从持股比例看，社保基金持有比例最多的是英科再生，持股量占流通股比例为11.69%，其次是比音勒芬，社保基金持股比例为10.08%，持股比例居前的还有常熟银行、浙江荣泰、云路股份等": {"topic": "金融", "similarity": 0.38363683223724365, "prompt": "新闻文本是从持股比例看，社保基金持有比例最多的是英科再生，持股量占流通股比例为11.69%，其次是比音勒芬，社保基金持股比例为10.08%，持股比例居前的还有常熟银行、浙江荣泰、云路股份等，包含的情绪词典是stock：0.0，financial：0.0"}, "持股数量方面，社保基金持股数量在1亿股以上的共有16只，社保基金持股量最多的是常熟银行，共持有2.90亿股，分众传媒、广汇能源等紧随其后，持股量分别为2.65亿股、2.14亿股": {"topic": "金融", "similarity": 0.4685646891593933, "prompt": "新闻文本是持股数量方面，社保基金持股数量在1亿股以上的共有16只，社保基金持股量最多的是常熟银行，共持有2.90亿股，分众传媒、广汇能源等紧随其后，持股量分别为2.65亿股、2.14亿股，包含的情绪词典是stock：0.0，finance：0.0"}, "（文章来源：证券时报网）": {"topic": null, "similarity": null, "prompt": "新闻文本是（文章来源：证券时报网），包含的情绪词典是stock：0.0，finance：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -855,7 +855,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，中信证券研报指出，2024年以来，家电内需渐入“地产竣工周期负反馈”": {"topic": "房地产", "similarity": 0.38335269689559937}, "较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期": {"topic": "宏观经济", "similarity": 0.4201096296310425}, "但上述逻辑预期，或阶段性构建家电板块交易性机会": {"topic": "金融", "similarity": 0.42112302780151367}}</t>
+          <t>{"证券时报网讯，中信证券研报指出，2024年以来，家电内需渐入“地产竣工周期负反馈”": {"topic": "房地产", "similarity": 0.38335269689559937, "prompt": "新闻文本是证券时报网讯，中信证券研报指出，2024年以来，家电内需渐入“地产竣工周期负反馈”，包含的情绪词典是necessitates：0.0，inflation：-0.5"}, "“以旧换新”政策适逢其时，用以对冲需求下行": {"topic": null, "similarity": null, "prompt": "新闻文本是“以旧换新”政策适逢其时，用以对冲需求下行，包含的情绪词典是policy：0.0，update：0.0"}, "较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期": {"topic": "宏观经济", "similarity": 0.4201095700263977, "prompt": "新闻文本是较为关键的是，本轮政策补贴力度较强，有希望在较大程度上平抑“家电价格战持续激化”以及“消费持续降级”的预期，包含的情绪词典是potential：0.3，strengthen：0.7"}, "缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力": {"topic": null, "similarity": null, "prompt": "新闻文本是缓解上市公司尤其是中小市值企业和中高端家电品类的盈利水平压力，包含的情绪词典是profitability：0.6，profitable：0.8"}, "“以旧换新”的政策成效仍需观察": {"topic": null, "similarity": null, "prompt": "新闻文本是“以旧换新”的政策成效仍需观察，包含的情绪词典是improvement：0.6，new：0.0"}, "但上述逻辑预期，或阶段性构建家电板块交易性机会": {"topic": "金融", "similarity": 0.42112302780151367, "prompt": "新闻文本是但上述逻辑预期，或阶段性构建家电板块交易性机会，包含的情绪词典是presumptively：0.0，presumably：0.0"}, "（文章来源：证券时报网）": {"topic": null, "similarity": null, "prompt": "新闻文本是（文章来源：证券时报网），包含的情绪词典是stock：0.0，finance：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>{"中国扩内需政策有望加码，叠加金九银十旺季，经济有望企稳": {"topic": "宏观经济", "similarity": 0.4764859676361084}, "重点关注：电子、非银金融、汽车、军工、家电、医药、互联网等": {"topic": "金融", "similarity": 0.5523044466972351}}</t>
+          <t>{"证券时报网讯，中信建投研报指出，经历数月回调后，9月市场有望边际改善": {"topic": null, "similarity": null, "prompt": "新闻文本是证券时报网讯，中信建投研报指出，经历数月回调后，9月市场有望边际改善，包含的情绪词典是stock：0.0，investment：0.4"}, "9月联储有望开启降息周期，流动性预期改善": {"topic": null, "similarity": null, "prompt": "新闻文本是9月联储有望开启降息周期，流动性预期改善，包含的情绪词典是inflation：-0.5，presumably：0.0"}, "中国扩内需政策有望加码，叠加金九银十旺季，经济有望企稳": {"topic": "宏观经济", "similarity": 0.4764859080314636, "prompt": "新闻文本是中国扩内需政策有望加码，叠加金九银十旺季，经济有望企稳，包含的情绪词典是economy：0.0，economic：0.0"}, "中报落地后，市场风险偏好有望边际改善": {"topic": null, "similarity": null, "prompt": "新闻文本是中报落地后，市场风险偏好有望边际改善，包含的情绪词典是risk：-0.4，risks：-0.4"}, "同时，整个过程预计渐进式改善，市场波动可能具有反复性，投资者需保持耐心，逐步伺机进攻": {"topic": null, "similarity": null, "prompt": "新闻文本是同时，整个过程预计渐进式改善，市场波动可能具有反复性，投资者需保持耐心，逐步伺机进攻，包含的情绪词典是improvement：0.6，process：0.0"}, "重点关注：电子、非银金融、汽车、军工、家电、医药、互联网等": {"topic": "金融", "similarity": 0.552304208278656, "prompt": "新闻文本是重点关注：电子、非银金融、汽车、军工、家电、医药、互联网等，包含的情绪词典是electronic：0.0，electrical：0.0"}, "（文章来源：证券时报网）": {"topic": null, "similarity": null, "prompt": "新闻文本是（文章来源：证券时报网），包含的情绪词典是stock：0.0，finance：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -965,7 +965,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>{"证券时报网讯，证券时报·数据宝统计显示，社保基金最新出现在66只科创板股前十大流通股东名单中，合计持股量2.85亿股，期末持股市值合计90.81亿元": {"topic": "金融", "similarity": 0.40915447473526}, "持股变动显示，新进19只，增持17只，减持9只，21只股持股量保持不变": {"topic": "金融", "similarity": 0.4507187604904175}, "新进股中，中国通号、珠海冠宇、莱特光电等持股量居前": {"topic": "金融", "similarity": 0.43083545565605164}, "持股数量方面，社保基金持股数量在1000万股以上的共有7只，社保基金持股量最多的是中国通号，共持有2988.26万股，西部超导、金宏气体等紧随其后，持股量分别为1521.76万股、1463.32万股": {"topic": "金融", "similarity": 0.4296455979347229}, "社保基金持股市值居前的有传音控股、西部超导、南微医学，持股市值分别为6.64亿元、5.83亿元、4.50亿元": {"topic": "金融", "similarity": 0.41091975569725037}}</t>
+          <t>{"证券时报网讯，证券时报·数据宝统计显示，社保基金最新出现在66只科创板股前十大流通股东名单中，合计持股量2.85亿股，期末持股市值合计90.81亿元": {"topic": "金融", "similarity": 0.40915438532829285, "prompt": "新闻文本是证券时报网讯，证券时报·数据宝统计显示，社保基金最新出现在66只科创板股前十大流通股东名单中，合计持股量2.85亿股，期末持股市值合计90.81亿元，包含的情绪词典是stock：0.0，fund：0.1"}, "持股变动显示，新进19只，增持17只，减持9只，21只股持股量保持不变": {"topic": "金融", "similarity": 0.4507187008857727, "prompt": "新闻文本是持股变动显示，新进19只，增持17只，减持9只，21只股持股量保持不变，包含的情绪词典是stock：0.0，hold：0.0"}, "新进股中，中国通号、珠海冠宇、莱特光电等持股量居前": {"topic": "金融", "similarity": 0.4308353364467621, "prompt": "新闻文本是新进股中，中国通号、珠海冠宇、莱特光电等持股量居前，包含的情绪词典是stock：0.0，investor：0.4"}, "社保基金持有科创板股中，从前十大流通股东名单中社保基金家数来看，社保基金家数最多的是英科再生，共有4家社保基金出现在前十大流通股东名单中，即易方达基金管理有限公司-社保基金17042组合、国泰基金管理有限公司-社保基金2103组合、全国社保基金一一一组合、易方达基金管理有限公司-社保基金17041组合，分别位列公司第三大、第五大、第六大、第十大流通股东，持股量合计为1196.97万股，占流通股比例为11.69%": {"topic": null, "similarity": null, "prompt": "新闻文本是社保基金持有科创板股中，从前十大流通股东名单中社保基金家数来看，社保基金家数最多的是英科再生，共有4家社保基金出现在前十大流通股东名单中，即易方达基金管理有限公司-社保基金17042组合、国泰基金管理有限公司-社保基金2103组合、全国社保基金一一一组合、易方达基金管理有限公司-社保基金17041组合，分别位列公司第三大、第五大、第六大、第十大流通股东，持股量合计为1196.97万股，占流通股比例为11.69%，包含的情绪词典是stock：0.0，innovation：0.7"}, "从持股比例看，社保基金持有比例最多的是英科再生，持股量占流通股比例为11.69%，其次是云路股份，社保基金持股比例为9.44%，持股比例居前的还有鼎阳科技、德科立、峰岹科技等": {"topic": null, "similarity": null, "prompt": "新闻文本是从持股比例看，社保基金持有比例最多的是英科再生，持股量占流通股比例为11.69%，其次是云路股份，社保基金持股比例为9.44%，持股比例居前的还有鼎阳科技、德科立、峰岹科技等，包含的情绪词典是stock：0.0，industry：0.0"}, "持股数量方面，社保基金持股数量在1000万股以上的共有7只，社保基金持股量最多的是中国通号，共持有2988.26万股，西部超导、金宏气体等紧随其后，持股量分别为1521.76万股、1463.32万股": {"topic": "金融", "similarity": 0.4296455383300781, "prompt": "新闻文本是持股数量方面，社保基金持股数量在1000万股以上的共有7只，社保基金持股量最多的是中国通号，共持有2988.26万股，西部超导、金宏气体等紧随其后，持股量分别为1521.76万股、1463.32万股，包含的情绪词典是stock：0.0，financial：0.0"}, "社保基金持股市值居前的有传音控股、西部超导、南微医学，持股市值分别为6.64亿元、5.83亿元、4.50亿元": {"topic": "金融", "similarity": 0.4109196662902832, "prompt": "新闻文本是社保基金持股市值居前的有传音控股、西部超导、南微医学，持股市值分别为6.64亿元、5.83亿元、4.50亿元，包含的情绪词典是stock：0.0，financial：0.0"}, "（文章来源：证券时报网）": {"topic": null, "similarity": null, "prompt": "新闻文本是（文章来源：证券时报网），包含的情绪词典是stock：0.0，finance：0.0"}}</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>{"SEC指控一家中国投资咨询公司涉嫌欺诈　　当地时间8月27日，美国SEC宣布指控总部位于中国的投资顾问公司QZ Asset、其位于美国南达科他州的控股公司QZ Global Limited以及两家公司的首席执行官Blake Yeung Pu Lei涉嫌欺诈": {"topic": "金融", "similarity": 0.3994976580142975}, "被控方在客户和潜在客户的投资安全、投资顾问公司与某些知名银行和律师事务所的关系，以及控股公司QZ Global的首次公开股票发行方面对客户和潜在客户撒谎": {"topic": "金融", "similarity": 0.376170814037323}, "根据指控，在实施了这一全球数百万美元的欺诈行为后，被告据称停止了与客户的沟通，客户用于访问其资金的QZ Asset网站也被关闭": {"topic": "金融", "similarity": 0.37470072507858276}, "涉事公司或为广州千泽投资　　美国SEC的公告显示，QZ Asset全称为Qianze Asset Management Limited": {"topic": "金融", "similarity": 0.394395112991333}, "公开信息显示，SEC所指的QZ Asset和Qianze Asset，或为广州千泽投资有限公司": {"topic": "金融", "similarity": 0.3946516811847687}, "公开信息显示，2019年，广州千泽资产管理有限公司（下称“千泽资管”）及其时任执行董事杨普磊进行了密集宣传，声称公司运用研发的“大数据+人工智能决策系统”（简称“BDAI”）为客户进行A股交易，收益良好": {"topic": "金融", "similarity": 0.4121772050857544}, "千泽资管官方微信公众号推文显示，“千泽资产的投顾产品可以让客户以极低资金更有效的运用在股市中，拥有更多的获利机会": {"topic": "金融", "similarity": 0.4502590298652649}, "对于那些尤其是喜欢短线操盘的投资者来说，智能操盘里的‘AI选股’等新型投顾产品将是不错的选择": {"topic": "金融", "similarity": 0.4615592360496521}, "（文章来源：上海证券报）": {"topic": "金融", "similarity": 0.3758732080459595}}</t>
+          <t>{"日前，美国证券交易委员会（SEC）披露了一则指控": {"topic": null, "similarity": null, "prompt": "新闻文本是日前，美国证券交易委员会（SEC）披露了一则指控，包含的情绪词典是sector：0.0，sentencing：0.0"}, "美国SEC宣布指控总部位于中国的投资顾问公司QZ Asset Management Limited（下称“QZ Asset”）、其位于美国南达科他州的控股公司QZ Global Limited（下称“QZ Global”）以及两家公司的首席执行官Blake Yeung Pu Lei（Yang Pulei，下称“Yeung”）涉嫌欺诈": {"topic": null, "similarity": null, "prompt": "新闻文本是美国SEC宣布指控总部位于中国的投资顾问公司QZ Asset Management Limited（下称“QZ Asset”）、其位于美国南达科他州的控股公司QZ Global Limited（下称“QZ Global”）以及两家公司的首席执行官Blake Yeung Pu Lei（Yang Pulei，下称“Yeung”）涉嫌欺诈，包含的情绪词典是chinese：0.0，investment：0.4"}, "SEC指控一家中国投资咨询公司涉嫌欺诈　　当地时间8月27日，美国SEC宣布指控总部位于中国的投资顾问公司QZ Asset、其位于美国南达科他州的控股公司QZ Global Limited以及两家公司的首席执行官Blake Yeung Pu Lei涉嫌欺诈": {"topic": "金融", "similarity": 0.39949771761894226, "prompt": "新闻文本是SEC指控一家中国投资咨询公司涉嫌欺诈　　当地时间8月27日，美国SEC宣布指控总部位于中国的投资顾问公司QZ Asset、其位于美国南达科他州的控股公司QZ Global Limited以及两家公司的首席执行官Blake Yeung Pu Lei涉嫌欺诈，包含的情绪词典是chinese：0.0，investment：0.4"}, "被控方在客户和潜在客户的投资安全、投资顾问公司与某些知名银行和律师事务所的关系，以及控股公司QZ Global的首次公开股票发行方面对客户和潜在客户撒谎": {"topic": "金融", "similarity": 0.3761707544326782, "prompt": "新闻文本是被控方在客户和潜在客户的投资安全、投资顾问公司与某些知名银行和律师事务所的关系，以及控股公司QZ Global的首次公开股票发行方面对客户和潜在客户撒谎，包含的情绪词典是investment：0.4，invest：0.3"}, "美国SEC的指控称，QZ Asset、QZ Global和Yeung骗取了数百人至少600万美元": {"topic": null, "similarity": null, "prompt": "新闻文本是美国SEC的指控称，QZ Asset、QZ Global和Yeung骗取了数百人至少600万美元，包含的情绪词典是several：0.0，investment：0.4"}, "根据指控，QZ Asset和Yeung谎称，QZ Asset将利用其基于人工智能的专有技术帮助客户每周获得超常回报，同时承诺“100%”保护客户资金，并称知名且信誉良好的金融和法律公司正在为该公司提供服务": {"topic": null, "similarity": null, "prompt": "新闻文本是根据指控，QZ Asset和Yeung谎称，QZ Asset将利用其基于人工智能的专有技术帮助客户每周获得超常回报，同时承诺“100%”保护客户资金，并称知名且信誉良好的金融和法律公司正在为该公司提供服务，包含的情绪词典是asset：0.3，investor：0.4"}, "指控还称，被告谎称QZ Global已申请其普通股在纳斯达克全球精选市场（Nasdaq Global Select Market）上市，并已与美国SEC的工作人员积极沟通": {"topic": null, "similarity": null, "prompt": "新闻文本是指控还称，被告谎称QZ Global已申请其普通股在纳斯达克全球精选市场（Nasdaq Global Select Market）上市，并已与美国SEC的工作人员积极沟通，包含的情绪词典是global：0.0，stock：0.0"}, "QZ Global吹嘘其已向美国SEC提交文件，以诱使客户和潜在客户将资金交给QZ Asset，但该文件存在重大缺陷": {"topic": null, "similarity": null, "prompt": "新闻文本是QZ Global吹嘘其已向美国SEC提交文件，以诱使客户和潜在客户将资金交给QZ Asset，但该文件存在重大缺陷，包含的情绪词典是asset：0.3，financial：0.0"}, "根据指控，在实施了这一全球数百万美元的欺诈行为后，被告据称停止了与客户的沟通，客户用于访问其资金的QZ Asset网站也被关闭": {"topic": "金融", "similarity": 0.3747006952762604, "prompt": "新闻文本是根据指控，在实施了这一全球数百万美元的欺诈行为后，被告据称停止了与客户的沟通，客户用于访问其资金的QZ Asset网站也被关闭，包含的情绪词典是asset：0.3，stoppage：-0.3"}, "美国SEC丹佛地区办公室地区总监Jason J. Burt表示：“被告公然的欺诈行为，包括他们滥用美国证券交易委员会的备案程序来欺诈美国和世界各地的投资者，应受到谴责": {"topic": null, "similarity": null, "prompt": "新闻文本是美国SEC丹佛地区办公室地区总监Jason J. Burt表示：“被告公然的欺诈行为，包括他们滥用美国证券交易委员会的备案程序来欺诈美国和世界各地的投资者，应受到谴责，包含的情绪词典是investor：0.4，case：0.0"}, "”美国SEC指控被告违反了联邦证券法的反欺诈条款，并将寻求永久禁制令、返还非法所得以及民事处罚": {"topic": null, "similarity": null, "prompt": "新闻文本是”美国SEC指控被告违反了联邦证券法的反欺诈条款，并将寻求永久禁制令、返还非法所得以及民事处罚，包含的情绪词典是law：0.0，legal：0.0"}, "涉事公司或为广州千泽投资　　美国SEC的公告显示，QZ Asset全称为Qianze Asset Management Limited": {"topic": "金融", "similarity": 0.3943951427936554, "prompt": "新闻文本是涉事公司或为广州千泽投资　　美国SEC的公告显示，QZ Asset全称为Qianze Asset Management Limited，包含的情绪词典是investment：0.4，invest：0.3"}, "公开信息显示，SEC所指的QZ Asset和Qianze Asset，或为广州千泽投资有限公司": {"topic": "金融", "similarity": 0.3946516811847687, "prompt": "新闻文本是公开信息显示，SEC所指的QZ Asset和Qianze Asset，或为广州千泽投资有限公司，包含的情绪词典是asset：0.3，investment：0.4"}, "其首席执行官Yang Pulei，其中文名字或为杨普磊": {"topic": null, "similarity": null, "prompt": "新闻文本是其首席执行官Yang Pulei，其中文名字或为杨普磊，包含的情绪词典是leader：0.6，leadership：0.7"}, "企查查信息显示，广州千泽投资有限公司成立于2012年，公司注册资本10000万元": {"topic": null, "similarity": null, "prompt": "新闻文本是企查查信息显示，广州千泽投资有限公司成立于2012年，公司注册资本10000万元，包含的情绪词典是company：0.0，investment：0.4"}, "2012年至2014年公司名为广州迈涛信息技术有限公司": {"topic": null, "similarity": null, "prompt": "新闻文本是2012年至2014年公司名为广州迈涛信息技术有限公司，包含的情绪词典是company：0.0，year：0.0"}, "2014年至2016年改名为广州优品资产管理有限公司": {"topic": null, "similarity": null, "prompt": "新闻文本是2014年至2016年改名为广州优品资产管理有限公司，包含的情绪词典是asset：0.3，investment：0.4"}, "2016年更名为广州千泽资产管理有限公司": {"topic": null, "similarity": null, "prompt": "新闻文本是2016年更名为广州千泽资产管理有限公司，包含的情绪词典是investment：0.4，invest：0.3"}, "2022年再度更名为广州千泽投资有限公司": {"topic": null, "similarity": null, "prompt": "新闻文本是2022年再度更名为广州千泽投资有限公司，包含的情绪词典是invest：0.3，investment：0.4"}, "目前公司已处于经营异常状态": {"topic": null, "similarity": null, "prompt": "新闻文本是目前公司已处于经营异常状态，包含的情绪词典是crisis：-0.8，company：0.0"}, "公开信息显示，2019年，广州千泽资产管理有限公司（下称“千泽资管”）及其时任执行董事杨普磊进行了密集宣传，声称公司运用研发的“大数据+人工智能决策系统”（简称“BDAI”）为客户进行A股交易，收益良好": {"topic": "金融", "similarity": 0.4121772050857544, "prompt": "新闻文本是公开信息显示，2019年，广州千泽资产管理有限公司（下称“千泽资管”）及其时任执行董事杨普磊进行了密集宣传，声称公司运用研发的“大数据+人工智能决策系统”（简称“BDAI”）为客户进行A股交易，收益良好，包含的情绪词典是trading：0.0，investor：0.4"}, "千泽资管官方微信公众号推文显示，“千泽资产的投顾产品可以让客户以极低资金更有效的运用在股市中，拥有更多的获利机会": {"topic": "金融", "similarity": 0.4502589702606201, "prompt": "新闻文本是千泽资管官方微信公众号推文显示，“千泽资产的投顾产品可以让客户以极低资金更有效的运用在股市中，拥有更多的获利机会，包含的情绪词典是invest：0.3，investment：0.4"}, "对于那些尤其是喜欢短线操盘的投资者来说，智能操盘里的‘AI选股’等新型投顾产品将是不错的选择": {"topic": "金融", "similarity": 0.46155911684036255, "prompt": "新闻文本是对于那些尤其是喜欢短线操盘的投资者来说，智能操盘里的‘AI选股’等新型投顾产品将是不错的选择，包含的情绪词典是investor：0.4，invest：0.3"}, "”千泽资管还曾售卖过一款名为“BDAI交易密钥”的产品": {"topic": null, "similarity": null, "prompt": "新闻文本是”千泽资管还曾售卖过一款名为“BDAI交易密钥”的产品，包含的情绪词典是trading：0.0，investor：0.4"}, "不过2019年10月31日之后，该公众号便停止更新": {"topic": null, "similarity": null, "prompt": "新闻文本是不过2019年10月31日之后，该公众号便停止更新，包含的情绪词典是stop：0.0，stoppage：-0.3"}, "（文章来源：上海证券报）": {"topic": "金融", "similarity": 0.3758731782436371, "prompt": "新闻文本是（文章来源：上海证券报），包含的情绪词典是stock：0.0，financial：0.0"}}</t>
         </is>
       </c>
     </row>

</xml_diff>